<commit_message>
update excelbook. on akj
</commit_message>
<xml_diff>
--- a/data/covidexcel.xlsx
+++ b/data/covidexcel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E9307F-2F6C-44FB-9D6F-413EDA07671D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E998AEF4-8371-43AE-A1DD-75767A0A725A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="735" windowWidth="20940" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="使い方" sheetId="6" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>NO</t>
   </si>
@@ -87,6 +87,72 @@
   </si>
   <si>
     <t>・</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>クエリ機能を有効にするため、以下の2つの許可が必要です。</t>
+    <rPh sb="3" eb="5">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>イカ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（セキュリティに不安がある場合、このファイルの利用を中止してください。）</t>
+  </si>
+  <si>
+    <t>「保護ビュー」</t>
+    <rPh sb="1" eb="3">
+      <t>ホゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「編集を有効にする」ボタンをクリックして編集を許可</t>
+    <rPh sb="20" eb="22">
+      <t>ヘンシュウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>キョカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「セキュリティの警告」</t>
+    <rPh sb="8" eb="10">
+      <t>ケイコク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「コンテンツの有効化」ボタンをクリックして外部データ接続を許可</t>
+    <rPh sb="7" eb="10">
+      <t>ユウコウカ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ガイブ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>キョカ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -510,7 +576,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB323F3-D0CB-43D7-B96B-6BCA940A5EF2}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -518,19 +584,69 @@
   <cols>
     <col min="1" max="1" width="3.375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.375" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="5"/>
+    <col min="3" max="3" width="3.625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.25" style="5" customWidth="1"/>
+    <col min="5" max="5" width="3.625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="6"/>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>